<commit_message>
adding barbosa query numbers
</commit_message>
<xml_diff>
--- a/EfficiencyResults.xlsx
+++ b/EfficiencyResults.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bfuller/Research/fhipe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{06891630-4A14-E14A-BD0E-A2987B05020A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7455F051-A8CF-4C40-B32C-53B68923C6E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="500" windowWidth="41840" windowHeight="28300"/>
+    <workbookView xWindow="9360" yWindow="500" windowWidth="41840" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EfficiencyResults" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Benchmarking Multi Basis Generation</t>
   </si>
@@ -87,11 +87,14 @@
   <si>
     <t>Enc DB Time Avg</t>
   </si>
+  <si>
+    <t> 0.5204222000747911</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -652,7 +655,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -665,14 +668,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Timing of Critical Operations for Different Values</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000" baseline="0"/>
               <a:t> of sigma</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2000"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -689,7 +692,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2035,6 +2038,9 @@
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>38.202514433860699</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>38.320589971542297</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2182,7 +2188,1248 @@
           <c:x val="0.52975980728202299"/>
           <c:y val="0.11643737144994079"/>
           <c:w val="0.47024019271797696"/>
-          <c:h val="4.4512496623937838E-2"/>
+          <c:h val="6.6833149814056886E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Size of Enc Database and Keys</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.37874904278390598"/>
+          <c:y val="1.7456359102244388E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EfficiencyResults!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Key size Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>EfficiencyResults!$A$2:$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>Number Bases</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Barbosa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EfficiencyResults!$F$3:$F$68</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>26796.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57406.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56527.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55618</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54738.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53837.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52962.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52071.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50283.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49402.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48499.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47612.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46732.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45823.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44930.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>44050.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43174.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42277.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41390</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40500.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39601.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>38719.4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37833.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>36931.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36037.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>35146.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>34262.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33373.800000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32471.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31589.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30698.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>29813.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>50634.8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>49063.3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>47502.7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45921.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>44351.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42790.3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41218.1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>39649.1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>38087.699999999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>36505.4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>34958.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>51704.3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>49254.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46810.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>44371.4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>41922.5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>56551.4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>53032.7</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>49519.3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>46024.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>57642.7</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>52874.3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>62643.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>71245.600000000006</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>78156.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>82680</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>84299.6</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>95519.4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>126154.6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>154346.9</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>224579.4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>422696.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>410003.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD89-6147-BDB3-9F1AF6CC3A91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EfficiencyResults!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Size Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>EfficiencyResults!$A$2:$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>Number Bases</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Barbosa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EfficiencyResults!$K$3:$K$68</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>5877550.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8657453.5999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8523196.8000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8388918.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8253989.5999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8118493.2000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7983286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7849134.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7714502.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7580157.2000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7445427.2000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7310501.5999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7176387.5999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7041544.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6907132.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6771624</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6636592</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6502150.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6367470.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6233300.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6098200.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5963836.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5828937.2000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5694382.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5559915.5999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5425216.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5289712.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5155209.2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5020238.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4885786.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4751508</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4616886</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4482159.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5781210.7999999998</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5602038</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5422521.5999999996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5241968.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5062829.2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4883446.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4703914.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4524648.8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4345002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4166027.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3985221.2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4746527.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4522256.4000000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4298308</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4073669.6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3849010.4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4340757.5999999996</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4071784.8</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3801836.8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3531835.6</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3800930.8</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3485847.2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3621308</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3664929.2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3619452</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3483413.6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3259390.4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3169130.4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3257465.6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3122308.8</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3076119.6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2984072.8</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2939307.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AD89-6147-BDB3-9F1AF6CC3A91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="515815295"/>
+        <c:axId val="565948959"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="515815295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="565948959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="565948959"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="10000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="515815295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.65773074022762745"/>
+          <c:y val="0.10506175506116601"/>
+          <c:w val="0.33341704224611124"/>
+          <c:h val="6.3166493215779454E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2259,6 +3506,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2814,6 +4101,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2847,6 +4650,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A89E789-6DE8-E746-A548-6C9211E32496}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3151,11 +4990,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z39" sqref="Z39"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6919,12 +8758,24 @@
       <c r="L68" s="1">
         <v>512.97033052604502</v>
       </c>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
+      <c r="M68" s="1">
+        <v>4.89842414855957E-2</v>
+      </c>
+      <c r="N68" s="1">
+        <v>3.3190645671518802E-3</v>
+      </c>
+      <c r="O68" s="1">
+        <v>38.320589971542297</v>
+      </c>
+      <c r="P68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>0</v>
+      </c>
+      <c r="R68" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>